<commit_message>
Updated instructions for next year
</commit_message>
<xml_diff>
--- a/Labs/Lab2/Assignment2Rubric.xlsx
+++ b/Labs/Lab2/Assignment2Rubric.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS246-CourseMaterials/Labs/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6F03D9-6D0E-7D45-835A-57C88C6B3F5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F483F83-F192-6648-AFB4-5EEEAA7C0689}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19160" yWindow="9920" windowWidth="17060" windowHeight="16440" activeTab="2" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17060" windowHeight="14720" activeTab="3" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 (4)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>Requirements</t>
   </si>
@@ -721,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00E69C9-CADA-6F47-B0B5-A6FB121FBF10}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D34"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -955,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E90A3F-7C6D-7841-BA3F-2EC4E92BA85F}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1149,4 +1150,165 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="5" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <f>SUM(B6:B14)</f>
+        <v>100</v>
+      </c>
+      <c r="C16" s="2">
+        <f>SUM(C6:C14)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added story quality to the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab2/Assignment2Rubric.xlsx
+++ b/Labs/Lab2/Assignment2Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5834FE-FAD9-2B40-B587-87C44886C9F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F26B016-5951-1147-9383-F00C9A9E7115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="500" windowWidth="10620" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="14760" yWindow="500" windowWidth="10620" windowHeight="14640" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Requirements</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Sprint 1 with 4+ stories</t>
+  </si>
+  <si>
+    <t>Stories written correctly</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD13E5-EC24-C14D-9BEE-EA2BBE4DEF6B}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -513,109 +516,120 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="5" customFormat="1">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="2">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2">
-        <f>SUM(B6:B14)</f>
+      <c r="B17" s="2">
+        <f>SUM(B6:B15)</f>
         <v>100</v>
       </c>
-      <c r="C16" s="2">
-        <f>SUM(C6:C14)</f>
+      <c r="C17" s="2">
+        <f>SUM(C6:C15)</f>
         <v>100</v>
       </c>
     </row>
@@ -626,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -674,109 +688,120 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="5" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="2">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2">
-        <f>SUM(B6:B14)</f>
+      <c r="B17" s="2">
+        <f>SUM(B6:B15)</f>
         <v>100</v>
       </c>
-      <c r="C16" s="2">
-        <f>SUM(C6:C14)</f>
+      <c r="C17" s="2">
+        <f>SUM(C6:C15)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New syllabus for 2024
</commit_message>
<xml_diff>
--- a/Labs/Lab2/Assignment2Rubric.xlsx
+++ b/Labs/Lab2/Assignment2Rubric.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS246-CourseMaterials\Labs\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F26B016-5951-1147-9383-F00C9A9E7115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391A5031-77AA-4FE0-AB0E-CF60EFE43135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="500" windowWidth="10620" windowHeight="14640" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="30612" yWindow="4080" windowWidth="23256" windowHeight="12576" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Requirements</t>
   </si>
@@ -77,13 +88,22 @@
   </si>
   <si>
     <t>Stories written correctly</t>
+  </si>
+  <si>
+    <t>3/5 assigned</t>
+  </si>
+  <si>
+    <t>only 2 stories</t>
+  </si>
+  <si>
+    <t>most are right</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -468,35 +488,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD13E5-EC24-C14D-9BEE-EA2BBE4DEF6B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,14 +527,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -522,10 +542,13 @@
         <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -536,7 +559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -547,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -558,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -569,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="5" customFormat="1">
+    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -580,14 +603,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -598,7 +621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -606,10 +629,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -617,10 +643,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -630,7 +659,7 @@
       </c>
       <c r="C17" s="2">
         <f>SUM(C6:C15)</f>
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -646,29 +675,29 @@
       <selection activeCell="A6" sqref="A6:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,14 +708,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -697,7 +726,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -719,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -730,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -741,7 +770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -752,14 +781,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="5" customFormat="1">
+    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -770,7 +799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -781,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -792,7 +821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added new overview doc
</commit_message>
<xml_diff>
--- a/Labs/Lab2/Assignment2Rubric.xlsx
+++ b/Labs/Lab2/Assignment2Rubric.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS246-CourseMaterials\Labs\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7421D533-8C3B-CD44-9C6D-CE84C763970A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B7ADFB-08CE-41BA-9457-D276C91F7799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="1340" windowWidth="13440" windowHeight="15320" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="38700" yWindow="5790" windowWidth="14985" windowHeight="13050" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Requirements</t>
   </si>
@@ -43,9 +54,6 @@
     <t>CS246 Assignment 2 Rubric</t>
   </si>
   <si>
-    <t>At least 20 user stories</t>
-  </si>
-  <si>
     <t>All stories have points</t>
   </si>
   <si>
@@ -67,9 +75,6 @@
     <t>At least 4 epics</t>
   </si>
   <si>
-    <t>At least 2 child stories per epic</t>
-  </si>
-  <si>
     <t>Backlog ordered by priority</t>
   </si>
   <si>
@@ -77,13 +82,40 @@
   </si>
   <si>
     <t>Stories written correctly</t>
+  </si>
+  <si>
+    <t>At least 2 user stories per epic</t>
+  </si>
+  <si>
+    <t>2+ sub-tasks for each story</t>
+  </si>
+  <si>
+    <t>Stories for all requirements</t>
+  </si>
+  <si>
+    <t>User stories for all requirements, min 7 per team member.</t>
+  </si>
+  <si>
+    <t>Lab 2 Requirements</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Summary report</t>
+  </si>
+  <si>
+    <t>Team contribution report</t>
+  </si>
+  <si>
+    <t>Your team did an excellent job on this lab. Your user stories are well written and you did a good job of adding them to epics. You did a good job of setting up the first sprint. There are just a couple issues which are noted below.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +158,17 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,13 +190,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,9 +231,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -212,7 +271,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -318,7 +377,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,35 +530,35 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.796875" customWidth="1"/>
+    <col min="2" max="2" width="9.296875" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,102 +567,102 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
         <v>30</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
+    <row r="7" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>20</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>8</v>
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" s="5" customFormat="1">
+    <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>8</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>8</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
         <v>8</v>
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -620,68 +679,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" customWidth="1"/>
+    <col min="2" max="2" width="8.796875" customWidth="1"/>
+    <col min="3" max="3" width="6.796875" customWidth="1"/>
+    <col min="4" max="4" width="1.5" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2">
-        <v>30</v>
-      </c>
-      <c r="C6" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D5" s="2"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
         <v>20</v>
@@ -689,105 +754,189 @@
       <c r="C7" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B15" s="2">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C16" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="D16" s="2"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="2"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
         <v>10</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C20" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="2">
-        <f>SUM(B6:B15)</f>
+      <c r="B23" s="2">
+        <f>SUM(B7:B21)</f>
         <v>100</v>
       </c>
-      <c r="C17" s="2">
-        <f>SUM(C6:C15)</f>
+      <c r="C23" s="2">
+        <f>SUM(C7:C21)</f>
         <v>100</v>
       </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>